<commit_message>
scripts 811 v005 y v006
</commit_message>
<xml_diff>
--- a/Competencia DAI/versiones datasets epic.xlsx
+++ b/Competencia DAI/versiones datasets epic.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jonathan\Desktop\MCD - Laboratorio\7.Labo_1\labo2021DAI\Competencia DAI\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DFB449CB-7619-46CD-AD57-9D0D268B7E6F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6889AB30-4607-45E9-91F0-3B4A49D979D9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{6AEAA8B6-1B14-4580-A93C-CDC9E3EEA61D}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>Versión dataset epic</t>
   </si>
@@ -73,6 +73,29 @@
   dataset[ foto_mes==201907,  Visa_fultimo_cierre   := NA ] 
   dataset[ foto_mes==202009,  Visa_fultimo_cierre   := NA ] 
 + valores en pesos DEFLACTADOS a precios de enero 2021</t>
+  </si>
+  <si>
+    <t>005</t>
+  </si>
+  <si>
+    <t>+ palancas TRUE: corregir, nuevasvars, lag1, delta1, lag2, delta2, ratiomax3, deflactar, canaritosimportancia
++ variables drift: "mpasivos_margen", "mactivos_margen", "mcuentas_saldo",
+                              "mcajeros_propios_descuentos", "mtarjeta_visa_descuentos",
+                              "mforex_sell", "mtransferencias_emitidas", 
+                              "Master_mfinanciacion_limite","Master_mconsumospesos",
+                              "Master_fultimo_cierre", "Master_madelantodolares","Master_mpagado",
+                              "Master_mpagominimo", "Master_mconsumototal", 
+                              "Visa_mfinanciacion_limite",
+                              "Visa_msaldototal", "Visa_msaldopesos", "Visa_msaldodolares",
+                              "Visa_mconsumospesos", "Visa_fultimo_cierre", "Visa_mconsumototal",
+                              "Visa_mpagominimo"
++ el resto es todo igual al 004</t>
+  </si>
+  <si>
+    <t>006</t>
+  </si>
+  <si>
+    <t>igual al 005 pero sin DEFLACTAR!</t>
   </si>
 </sst>
 </file>
@@ -116,7 +139,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
@@ -124,17 +147,20 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
       <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -450,10 +476,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2FD619B1-66C5-4878-90DA-9F593933E3D0}">
-  <dimension ref="A1:I5"/>
+  <dimension ref="A1:I7"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5:I5"/>
+    <sheetView tabSelected="1" topLeftCell="A6" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -466,12 +492,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A1" s="5" t="s">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="4" t="s">
         <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
@@ -479,13 +505,13 @@
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3" s="2"/>
+      <c r="A3" s="4"/>
       <c r="B3" s="1" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A4" s="3" t="s">
+      <c r="A4" s="2" t="s">
         <v>2</v>
       </c>
       <c r="B4" s="1" t="s">
@@ -493,24 +519,48 @@
       </c>
     </row>
     <row r="5" spans="1:9" ht="308.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="3" t="s">
+      <c r="A5" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B5" s="6" t="s">
+      <c r="B5" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="C5" s="4"/>
-      <c r="D5" s="4"/>
-      <c r="E5" s="4"/>
-      <c r="F5" s="4"/>
-      <c r="G5" s="4"/>
-      <c r="H5" s="4"/>
-      <c r="I5" s="4"/>
+      <c r="C5" s="6"/>
+      <c r="D5" s="6"/>
+      <c r="E5" s="6"/>
+      <c r="F5" s="6"/>
+      <c r="G5" s="6"/>
+      <c r="H5" s="6"/>
+      <c r="I5" s="6"/>
+    </row>
+    <row r="6" spans="1:9" ht="221.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C6" s="5"/>
+      <c r="D6" s="5"/>
+      <c r="E6" s="5"/>
+      <c r="F6" s="5"/>
+      <c r="G6" s="5"/>
+      <c r="H6" s="5"/>
+      <c r="I6" s="5"/>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A7" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>11</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="3">
     <mergeCell ref="A2:A3"/>
     <mergeCell ref="B5:I5"/>
+    <mergeCell ref="B6:I6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
scripts dataset 7 8 y 9
</commit_message>
<xml_diff>
--- a/Competencia DAI/versiones datasets epic.xlsx
+++ b/Competencia DAI/versiones datasets epic.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jonathan\Desktop\MCD - Laboratorio\7.Labo_1\labo2021DAI\Competencia DAI\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2122A612-C99F-457C-8D3B-BBEC04333B60}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3FCC1B4E-3A8D-47A9-94ED-613229908B0F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{6AEAA8B6-1B14-4580-A93C-CDC9E3EEA61D}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
   <si>
     <t>Versión dataset epic</t>
   </si>
@@ -108,6 +108,12 @@
   </si>
   <si>
     <t>el 005 con tendencia</t>
+  </si>
+  <si>
+    <t>009</t>
+  </si>
+  <si>
+    <t>el 006 con tendencia</t>
   </si>
 </sst>
 </file>
@@ -488,10 +494,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2FD619B1-66C5-4878-90DA-9F593933E3D0}">
-  <dimension ref="A1:I9"/>
+  <dimension ref="A1:I10"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A6" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -584,6 +590,14 @@
         <v>15</v>
       </c>
     </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A10" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="3">
     <mergeCell ref="A2:A3"/>

</xml_diff>